<commit_message>
Fixed major bugs in MyCam
</commit_message>
<xml_diff>
--- a/Matlab Ver/Template.xlsx
+++ b/Matlab Ver/Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Matlab Workspace\Project Cams\GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Matlab Workspace\Git Backed\cam-profile-coord-gen\Matlab Ver\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>CW/CCW:</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>RISE</t>
-  </si>
-  <si>
-    <t>DWELL</t>
-  </si>
-  <si>
-    <t>FALL</t>
   </si>
   <si>
     <t>UV</t>
@@ -453,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3"/>
     </row>
@@ -526,97 +520,55 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1">
         <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
       </c>
       <c r="D10" s="1">
         <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>